<commit_message>
updated for Lesson 13 Project
</commit_message>
<xml_diff>
--- a/Decision Rules.xlsx
+++ b/Decision Rules.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bottl\Documents\DevMtnQLH4\Automation\lesson12Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bottl\Documents\DevMtnQLH4\Automation\homeLoanWizard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C1660F8-A1F0-4590-AF56-7530820BB58F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB59B0C-87AF-47D7-95A3-E8495D21A839}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3960" yWindow="468" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blank Template" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Title:</t>
   </si>
@@ -56,6 +56,27 @@
   </si>
   <si>
     <t>Large Down</t>
+  </si>
+  <si>
+    <t>Has Been Bankrupt</t>
+  </si>
+  <si>
+    <t>Has Had Foreclosure</t>
+  </si>
+  <si>
+    <t>Reject Application</t>
+  </si>
+  <si>
+    <t>Counseling Referral</t>
+  </si>
+  <si>
+    <t>Case 5</t>
+  </si>
+  <si>
+    <t>Case 6</t>
+  </si>
+  <si>
+    <t>Case 7</t>
   </si>
 </sst>
 </file>
@@ -103,7 +124,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -307,6 +328,26 @@
       <right style="thick">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
       <top/>
       <bottom style="thick">
         <color rgb="FF000000"/>
@@ -317,7 +358,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -355,11 +396,28 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF3F3F3"/>
+          <bgColor rgb="FFF3F3F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF000000"/>
@@ -684,10 +742,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -695,7 +753,7 @@
     <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -704,9 +762,12 @@
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
       <c r="B2" s="5" t="s">
         <v>1</v>
@@ -717,100 +778,255 @@
       <c r="D2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="F2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
-      <c r="E3" s="9"/>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="9"/>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="C4" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="E4" s="12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="B6" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="C5" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="D5" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" s="12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="B7" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="15"/>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="15"/>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="C9" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="F9" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="C10" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="C7" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="D7" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="E7" s="12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
+      <c r="B11" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C11" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F11" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="G11" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="C8" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="D8" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="E8" s="20" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="B12" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="C12" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="F12" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="G12" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12" s="20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <conditionalFormatting sqref="A4:E5 A7:E8">
-    <cfRule type="expression" dxfId="0" priority="1">
+  <conditionalFormatting sqref="A9:H12 A4:H7">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>